<commit_message>
trying to change the file to .gpkg and failing. Needs correction. Corrected files data.
</commit_message>
<xml_diff>
--- a/Bezrobocie.xlsx
+++ b/Bezrobocie.xlsx
@@ -8,85 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EconometricsProject\Spacial-Econometrics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6092D067-71AF-4C56-8BF4-6A6B9054CB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C76AE32-95DA-4DEA-B270-CF26C156FF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="37" windowWidth="16200" windowHeight="9308" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabl. 3(27)" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tabl. 3(27)'!$B$1:$C$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tabl. 3(27)'!$B$1:$B$21</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">Słupsk  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">gdański  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kartuski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">nowodworski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pucki  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">wejherowski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bytowski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">chojnicki  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">człuchowski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lęborski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">słupski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kościerski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kwidzyński  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">malborski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">starogardzki  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sztumski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tczewski  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gdańsk  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gdynia  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sopot  </t>
-  </si>
-  <si>
-    <t>County</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Unemployment</t>
   </si>
@@ -496,15 +433,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -846,253 +780,189 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.1328125" style="2"/>
-    <col min="2" max="2" width="20.73046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="14.73046875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>22</v>
+    <row r="1" spans="1:2" ht="36" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A2" s="5">
         <v>2201</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="4">
         <v>2907</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A3" s="6">
+    <row r="3" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A3" s="5">
         <v>2202</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="4">
         <v>3213</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A4" s="6">
+    <row r="4" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A4" s="5">
         <v>2203</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4">
         <v>1883</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A5" s="6">
+    <row r="5" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A5" s="5">
         <v>2204</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4">
         <v>1718</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A6" s="6">
+    <row r="6" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A6" s="5">
         <v>2205</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4">
         <v>1490</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A7" s="6">
+    <row r="7" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A7" s="5">
         <v>2206</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4">
         <v>1829</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A8" s="6">
+    <row r="8" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A8" s="5">
         <v>2207</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="4">
         <v>1720</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A9" s="6">
+    <row r="9" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A9" s="5">
         <v>2208</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="4">
         <v>1899</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A10" s="6">
+    <row r="10" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A10" s="5">
         <v>2209</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4">
         <v>2203</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A11" s="6">
+    <row r="11" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A11" s="5">
         <v>2210</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="4">
         <v>1500</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A12" s="6">
+    <row r="12" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A12" s="5">
         <v>2211</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4">
         <v>1950</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A13" s="6">
+    <row r="13" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A13" s="5">
         <v>2212</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="4">
         <v>2289</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A14" s="6">
+    <row r="14" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A14" s="5">
         <v>2213</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="4">
         <v>2508</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A15" s="6">
+    <row r="15" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A15" s="5">
         <v>2214</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="4">
         <v>2815</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A16" s="6">
+    <row r="16" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A16" s="5">
         <v>2215</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="4">
         <v>3999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A17" s="6">
+    <row r="17" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A17" s="5">
         <v>2216</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="4">
         <v>1113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A18" s="6">
+    <row r="18" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A18" s="5">
         <v>2261</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="4">
         <v>6552</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A19" s="6">
+    <row r="19" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A19" s="5">
         <v>2262</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B19" s="4">
         <v>2779</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A20" s="6">
+    <row r="20" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A20" s="5">
         <v>2263</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="B20" s="4">
         <v>1369</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="9.9499999999999993" customHeight="1">
-      <c r="A21" s="6">
+    <row r="21" spans="1:2" ht="9.9499999999999993" customHeight="1">
+      <c r="A21" s="5">
         <v>2264</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="4">
         <v>346</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>